<commit_message>
Edited the test files because some of them were wrong; ran all the tests again and updated TestResultsInOneFile
</commit_message>
<xml_diff>
--- a/src/TestResults/TestResultsInOneFile.xlsx
+++ b/src/TestResults/TestResultsInOneFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esther\Documents\CPSC433\Assignment\src\TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{57A44A3B-B16D-469B-89FB-25CDA1510A3B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{645695FF-EED6-475C-ADBC-90AFB41642AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{65AC3189-960A-4156-81B1-8C7E880493C9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>Input File</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Memo</t>
   </si>
   <si>
-    <t>Shouldn't it be Invalid course slots data</t>
-  </si>
-  <si>
     <t>Shouldn't it be Invalid labs slots data</t>
   </si>
   <si>
@@ -170,11 +167,6 @@
   </si>
   <si>
     <t>EveningClass</t>
-  </si>
-  <si>
-    <t>Eval-value: 0.0
-CPSC 916 LEC 01             : TU, 8:00
-CPSC 918 LEC 01             : MO, 19:00</t>
   </si>
   <si>
     <t>The results are wrong; evening courses can only be assigned to evening slots</t>
@@ -215,10 +207,22 @@
     <t>The results are wrong; it is possible to assign any class to an evening slot. It's just that evening classes must be assigned to evening slots.</t>
   </si>
   <si>
-    <t>It seems like this test failed because the program doesn't allow normal classes to be assgined to evening slots. However, they can be; so the reason should be NO VALID SOLUTION, not Invalid Course Slots Data</t>
-  </si>
-  <si>
     <t>CPSC913and413</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 333 LEC 01             : TU, 18:30</t>
+  </si>
+  <si>
+    <t>The results are wrong; CPSC 813 should be assigned to TU 18:00 and CPSC 313 should be assigned to MO 9:00.</t>
+  </si>
+  <si>
+    <t>The results are wrong; CPSC 913 should be assigned to TU 18:00 and CPSC 413 should be assigned to MO 10:00.</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 416 LEC 09             : TU, 8:00
+CPSC 518 LEC 09             : MO, 19:00</t>
   </si>
 </sst>
 </file>
@@ -242,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +256,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -296,6 +306,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,7 +629,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,13 +651,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>36</v>
@@ -651,7 +665,7 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>23</v>
@@ -662,13 +676,13 @@
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -704,18 +718,18 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="9" t="s">
         <v>57</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -764,7 +778,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -775,10 +789,10 @@
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>25</v>
@@ -789,21 +803,21 @@
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
@@ -812,33 +826,33 @@
         <v>25</v>
       </c>
       <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="F15" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,35 +935,32 @@
         <v>28</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="4" t="s">
+      <c r="B25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -965,18 +976,18 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>25</v>
+      <c r="D28" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Added Jorg's example files and re-ran the tests after the most recent changes to the code
</commit_message>
<xml_diff>
--- a/src/TestResults/TestResultsInOneFile.xlsx
+++ b/src/TestResults/TestResultsInOneFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esther\Documents\CPSC433\Assignment\src\TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{645695FF-EED6-475C-ADBC-90AFB41642AD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1FA1A15-EE7B-40DE-9A8F-1289AC68900C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{65AC3189-960A-4156-81B1-8C7E880493C9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
   <si>
     <t>Input File</t>
   </si>
@@ -121,13 +121,6 @@
   </si>
   <si>
     <t>PartAssign2</t>
-  </si>
-  <si>
-    <t>Eval-value: 1.0
-CPSC 433 LEC 01             : TU, 9:30
-CPSC 433 LEC 02             : TU, 9:30
-CPSC 433 TUT 01             : TU, 12:00
-CPSC 433 LAB 02             : TU, 12:00</t>
   </si>
   <si>
     <t>Eval-value: 0.0
@@ -145,9 +138,6 @@
     <t>Memo</t>
   </si>
   <si>
-    <t>Shouldn't it be Invalid labs slots data</t>
-  </si>
-  <si>
     <t>Not too sure what the output should be; this example is directly from Jorg's website</t>
   </si>
   <si>
@@ -178,23 +168,12 @@
     <t>500LevelCourses2</t>
   </si>
   <si>
-    <t>Eval-value: 0.0
-CPSC 516 LEC 01             : TU, 8:00
-CPSC 518 LEC 01             : MO, 8:00
-CPSC 354 LEC 01             : MO, 8:00</t>
-  </si>
-  <si>
     <t>Tuesdays1100to1230</t>
   </si>
   <si>
     <t>CPSC813and913</t>
   </si>
   <si>
-    <t>Eval-value: 0.0
-CPSC 913 LEC 01             : MO, 18:00
-CPSC 813 LEC 01             : MO, 18:00</t>
-  </si>
-  <si>
     <t>The results are wrong; CPSC 813 and 913 can only be assigned to TU 18:00-19:00</t>
   </si>
   <si>
@@ -202,9 +181,6 @@
   </si>
   <si>
     <t>AssignNormalClassToEveningSlot</t>
-  </si>
-  <si>
-    <t>The results are wrong; it is possible to assign any class to an evening slot. It's just that evening classes must be assigned to evening slots.</t>
   </si>
   <si>
     <t>CPSC913and413</t>
@@ -223,6 +199,123 @@
     <t>Eval-value: 0.0
 CPSC 416 LEC 09             : TU, 8:00
 CPSC 518 LEC 09             : MO, 19:00</t>
+  </si>
+  <si>
+    <t>CPSC313</t>
+  </si>
+  <si>
+    <t>ERROR: CPSC 813 cannot be initialized due to TU 18:00 lab slot never being defined.
+NO VALID SOLUTION</t>
+  </si>
+  <si>
+    <t>CPSC413</t>
+  </si>
+  <si>
+    <t>ERROR: CPSC 913 cannot be initialized due to TU 18:00 lab slot never being defined.
+NO VALID SOLUTION</t>
+  </si>
+  <si>
+    <t>gehtnicht1</t>
+  </si>
+  <si>
+    <t>gehtnicht2</t>
+  </si>
+  <si>
+    <t>gehtnicht3</t>
+  </si>
+  <si>
+    <t>gehtnicht4</t>
+  </si>
+  <si>
+    <t>gehtnicht5</t>
+  </si>
+  <si>
+    <t>gehtnicht6</t>
+  </si>
+  <si>
+    <t>gehtnicht7</t>
+  </si>
+  <si>
+    <t>gehtnicht8</t>
+  </si>
+  <si>
+    <t>gehtnicht9</t>
+  </si>
+  <si>
+    <t>gehtnicht10</t>
+  </si>
+  <si>
+    <t>gehtnicht11</t>
+  </si>
+  <si>
+    <t>gehtnicht12</t>
+  </si>
+  <si>
+    <t>pairing</t>
+  </si>
+  <si>
+    <t>parallelpen</t>
+  </si>
+  <si>
+    <t>prefexamp</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 354 LEC 01             : MO, 8:00
+CPSC 516 LEC 01             : TU, 8:00
+CPSC 518 LEC 01             : MO, 8:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 5.0
+CPSC 101 LEC 01             : MO, 8:00
+CPSC 102 LEC 01             : MO, 9:00
+CPSC 103 LEC 01             : MO, 9:00
+CPSC 104 LEC 01             : MO, 10:00
+CPSC 105 LEC 01             : MO, 10:00
+CPSC 106 LEC 01             : MO, 10:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 1.0
+CPSC 101 LEC 01             : MO, 10:00
+CPSC 101 LEC 02             : MO, 10:00
+CPSC 101 LEC 03             : MO, 9:00
+CPSC 101 LEC 04             : MO, 8:00
+CPSC 102 LEC 01             : MO, 10:00
+CPSC 102 LEC 02             : MO, 9:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 1.0
+CPSC 433 LAB 02             : TU, 12:00
+CPSC 433 LEC 01             : TU, 9:30
+CPSC 433 LEC 02             : TU, 9:30
+CPSC 433 TUT 01             : TU, 12:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 30.0
+CPSC 101 LEC 01             : MO, 8:00
+CPSC 102 LEC 01             : MO, 10:00
+CPSC 103 LEC 01             : MO, 9:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 313 LEC 01             : MO, 9:00
+CPSC 813 LEC 01             : TU, 18:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 3.0
+CPSC 433 LEC 01             : MO, 9:00
+CPSC 433 LEC 01 TUT 01      : TU, 10:00
+CPSC 433 LEC 02             : TU, 9:30
+CPSC 433 LEC 02 LAB 02      : MO, 8:00
+CPSC 567 LEC 01             : MO, 8:00
+CPSC 567 TUT 01             : FR, 10:00
+SENG 311 LEC 01             : MO, 8:00
+SENG 311 LEC 01 TUT 01      : FR, 10:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 813 LEC 01             : MO, 18:00
+CPSC 913 LEC 01             : MO, 18:00</t>
   </si>
 </sst>
 </file>
@@ -293,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -310,6 +403,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -626,21 +722,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42644B4F-7B93-4119-888A-47B71841FFC0}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="79" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="72.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="124.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
@@ -651,21 +748,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>23</v>
@@ -676,13 +773,13 @@
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>24</v>
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,16 +817,13 @@
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -740,7 +834,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -778,7 +872,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
@@ -787,160 +881,159 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="4" t="s">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>49</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="5"/>
       <c r="F15" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="5" t="s">
+    <row r="19" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="B20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>23</v>
@@ -948,10 +1041,11 @@
       <c r="D25" s="8" t="s">
         <v>28</v>
       </c>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>23</v>
@@ -959,68 +1053,71 @@
       <c r="D26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>23</v>
@@ -1029,9 +1126,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>23</v>
@@ -1040,14 +1137,208 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" s="9"/>
+    </row>
+    <row r="41" spans="1:7" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some more test files and edited the results
</commit_message>
<xml_diff>
--- a/src/TestResults/TestResultsInOneFile.xlsx
+++ b/src/TestResults/TestResultsInOneFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esther\Documents\CPSC433\Assignment\src\TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1FA1A15-EE7B-40DE-9A8F-1289AC68900C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B9F4BEB-C538-4A44-AF9B-478E14AE28FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{65AC3189-960A-4156-81B1-8C7E880493C9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
   <si>
     <t>Input File</t>
   </si>
@@ -316,6 +316,47 @@
     <t>Eval-value: 0.0
 CPSC 813 LEC 01             : MO, 18:00
 CPSC 913 LEC 01             : MO, 18:00</t>
+  </si>
+  <si>
+    <t>Incompatible</t>
+  </si>
+  <si>
+    <t>Unwanted</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 433 LEC 01             : MO, 8:00</t>
+  </si>
+  <si>
+    <t>Preferences</t>
+  </si>
+  <si>
+    <t>Eval-value: 20.0
+CPSC 433 LAB 02             : MO, 11:00
+CPSC 433 LEC 01             : MO, 10:00
+CPSC 433 LEC 02             : MO, 8:00
+CPSC 433 TUT 01             : TU, 10:00</t>
+  </si>
+  <si>
+    <t>Pair</t>
+  </si>
+  <si>
+    <t>Eval-value: 1.0
+CPSC 433 LEC 01             : MO, 10:00
+CPSC 433 LEC 02             : MO, 10:00</t>
+  </si>
+  <si>
+    <t>InvalidTimeSlot</t>
+  </si>
+  <si>
+    <t>JustLab</t>
+  </si>
+  <si>
+    <t>ERROR: lab/tutorial defined without any lecture section for their shared class identifier, CPSC 433 LAB 01
+Error: Invalid labs data</t>
+  </si>
+  <si>
+    <t>BiggerMinThanMax</t>
   </si>
 </sst>
 </file>
@@ -722,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42644B4F-7B93-4119-888A-47B71841FFC0}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,166 +867,166 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>57</v>
+      <c r="D13" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="4" t="s">
+      <c r="E18" s="5"/>
+      <c r="F18" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="B20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>23</v>
@@ -997,7 +1038,7 @@
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>23</v>
@@ -1009,7 +1050,7 @@
     </row>
     <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>23</v>
@@ -1021,7 +1062,7 @@
     </row>
     <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>23</v>
@@ -1033,7 +1074,7 @@
     </row>
     <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>23</v>
@@ -1045,7 +1086,7 @@
     </row>
     <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>23</v>
@@ -1057,7 +1098,7 @@
     </row>
     <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>23</v>
@@ -1069,276 +1110,357 @@
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="B29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="B30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="2" t="s">
+      <c r="B36" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A37" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="G40" s="9"/>
-    </row>
-    <row r="41" spans="1:7" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>28</v>
+        <v>73</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" s="4" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="B51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="2" t="s">
+      <c r="B55" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="2" t="s">
+      <c r="B56" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C50" s="2" t="s">
+      <c r="B57" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Edited the test files, for some of them were not valid
</commit_message>
<xml_diff>
--- a/src/TestResults/TestResultsInOneFile.xlsx
+++ b/src/TestResults/TestResultsInOneFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esther\Documents\CPSC433\Assignment\src\TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B9F4BEB-C538-4A44-AF9B-478E14AE28FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3B73D36B-CF55-48F5-BB66-7E8D2432F10F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{65AC3189-960A-4156-81B1-8C7E880493C9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="94">
   <si>
     <t>Input File</t>
   </si>
@@ -159,9 +159,6 @@
     <t>EveningClass</t>
   </si>
   <si>
-    <t>The results are wrong; evening courses can only be assigned to evening slots</t>
-  </si>
-  <si>
     <t>500LevelCourses1</t>
   </si>
   <si>
@@ -196,16 +193,7 @@
     <t>The results are wrong; CPSC 913 should be assigned to TU 18:00 and CPSC 413 should be assigned to MO 10:00.</t>
   </si>
   <si>
-    <t>Eval-value: 0.0
-CPSC 416 LEC 09             : TU, 8:00
-CPSC 518 LEC 09             : MO, 19:00</t>
-  </si>
-  <si>
     <t>CPSC313</t>
-  </si>
-  <si>
-    <t>ERROR: CPSC 813 cannot be initialized due to TU 18:00 lab slot never being defined.
-NO VALID SOLUTION</t>
   </si>
   <si>
     <t>CPSC413</t>
@@ -357,6 +345,21 @@
   </si>
   <si>
     <t>BiggerMinThanMax</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 313 LEC 01             : MO, 9:00
+CPSC 813 LAB 01             : TU, 18:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 413 LEC 01             : MO, 9:00
+CPSC 913 LAB 01             : TU, 18:00</t>
+  </si>
+  <si>
+    <t>Eval-value: 0.0
+CPSC 416 LEC 90             : MO, 19:00
+CPSC 518 LEC 91             : MO, 19:00</t>
   </si>
 </sst>
 </file>
@@ -427,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -447,6 +450,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -765,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42644B4F-7B93-4119-888A-47B71841FFC0}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,7 +810,7 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>23</v>
@@ -814,13 +821,13 @@
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -858,18 +865,18 @@
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>23</v>
@@ -934,59 +941,55 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>23</v>
@@ -996,7 +999,7 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1010,23 +1013,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:6" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>43</v>
+      <c r="B20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>23</v>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>23</v>
@@ -1050,7 +1050,7 @@
     </row>
     <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>23</v>
@@ -1062,7 +1062,7 @@
     </row>
     <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>23</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>23</v>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>23</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>23</v>
@@ -1110,7 +1110,7 @@
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>23</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>23</v>
@@ -1134,19 +1134,19 @@
     </row>
     <row r="30" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>23</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>23</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>23</v>
@@ -1182,7 +1182,7 @@
     </row>
     <row r="34" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>23</v>
@@ -1194,13 +1194,13 @@
     </row>
     <row r="35" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E35" s="9"/>
     </row>
@@ -1250,35 +1250,35 @@
     </row>
     <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1289,7 +1289,7 @@
         <v>24</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,24 +1305,24 @@
     </row>
     <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G46" s="9"/>
     </row>
@@ -1337,7 +1337,7 @@
         <v>34</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>36</v>
@@ -1378,7 +1378,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>23</v>
@@ -1389,13 +1389,13 @@
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>